<commit_message>
keep trip data for distribution
</commit_message>
<xml_diff>
--- a/distribution/example-data-and-results/input/trips-checklists-trip-reports.xlsx
+++ b/distribution/example-data-and-results/input/trips-checklists-trip-reports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63ef30ccc6dfe22d/Documents/WOS-WFO-2025-Conference/Birdlist-compilation-20250715/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick_paulson/Documents/home/storage/CloudStation/git-repo-collection/working-dirs/org/3rivers-ashtanga/2013/wos-ebird-summary/distribution/example-data-and-results/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="618" documentId="8_{C5A86F08-7017-3946-9AF2-F77D101C259C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59259772-9CE1-1944-94F5-42AA5575AAD9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9E0921-41E3-7643-8141-5C9F4B7CF41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="760" windowWidth="25720" windowHeight="18560" xr2:uid="{59813396-17C2-6944-A7F1-1C753F589504}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="267">
   <si>
     <t>Ahtanum</t>
   </si>
@@ -190,12 +190,6 @@
     <t>Miles McEvoy</t>
   </si>
   <si>
-    <t>Trip Reports</t>
-  </si>
-  <si>
-    <t>Checklists</t>
-  </si>
-  <si>
     <t>Trip Key</t>
   </si>
   <si>
@@ -287,12 +281,6 @@
   </si>
   <si>
     <t>Mike &amp; MerryLynn Denny</t>
-  </si>
-  <si>
-    <t>https://ebird.org/checklist/S247867506</t>
-  </si>
-  <si>
-    <t>https://ebird.org/tripreport/382648</t>
   </si>
   <si>
     <t>Tim O'Brien</t>
@@ -854,226 +842,22 @@
     <t>https://ebird.org/checklist/S247781044</t>
   </si>
   <si>
-    <t>Trip Report Compilation Output</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-2.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-3.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-4.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-5.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-6.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-7.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-8.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-9.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-10.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-11.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-12.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-13.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-14.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-15.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-16.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-17.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-18.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-19.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-20.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-21.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-22.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-23.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-24.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-25.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-26.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-27.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-28.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-29.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-30.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-31.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-32.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-33.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-34.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-35.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-36.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-37.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-39.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-40.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-41.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-42.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-43.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-44.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-45.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-46.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-47.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-48.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-51.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-52.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-53.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-54.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-55.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-56.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-57.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-58.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-59.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-60.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-61.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-62.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-63.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-64.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-65.xlsx</t>
-  </si>
-  <si>
     <t>Lauren Smith</t>
   </si>
   <si>
     <t>https://ebird.org/tripreport/382208</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-66.xlsx</t>
-  </si>
-  <si>
     <t>Deb Esman?</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-67.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-68.xlsx</t>
-  </si>
-  <si>
     <t>https://ebird.org/tripreport/387079</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-69.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-70.xlsx</t>
-  </si>
-  <si>
     <t>Bruce LaBar</t>
   </si>
   <si>
     <t>https://ebird.org/tripreport/382173</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-71.xlsx</t>
   </si>
   <si>
     <t>https://ebird.org/checklist/S248682413
@@ -1083,22 +867,10 @@
 https://ebird.org/checklist/S248683659</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-72.xlsx</t>
-  </si>
-  <si>
     <t>https://ebird.org/tripreport/383166</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-73.xlsx</t>
-  </si>
-  <si>
     <t>https://ebird.org/checklist/S247195427</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-74.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-75.xlsx</t>
   </si>
   <si>
     <t>S247582618
@@ -1107,12 +879,6 @@
 S247582838</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-76.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-77.xlsx</t>
-  </si>
-  <si>
     <t>Coming Over:
 North Seattle / Snohomish Co</t>
   </si>
@@ -1134,10 +900,23 @@
     <t>https://ebird.org/tripreport/383154</t>
   </si>
   <si>
-    <t>CompiledSpreadsheet-78.xlsx</t>
-  </si>
-  <si>
-    <t>CompiledSpreadsheet-79.xlsx</t>
+    <t>Trip Reports/Checklists</t>
+  </si>
+  <si>
+    <t>https://ebird.org/tripreport/382648
+https://ebird.org/checklist/S247867506</t>
+  </si>
+  <si>
+    <t>https://ebird.org/tripreport/394588</t>
+  </si>
+  <si>
+    <t>https://ebird.org/tripreport/387050</t>
+  </si>
+  <si>
+    <t>https://ebird.org/tripreport/387044</t>
+  </si>
+  <si>
+    <t>https://ebird.org/tripreport/384698</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1021,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1295,11 +1074,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1307,13 +1083,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{7CD75048-BFDF-7F4F-84AC-906C52B281AE}"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1381,23 +1151,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D043231-9B53-AA48-9D06-6F5D5240F721}" name="Table2" displayName="Table2" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J79" xr:uid="{9D043231-9B53-AA48-9D06-6F5D5240F721}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D043231-9B53-AA48-9D06-6F5D5240F721}" name="Table2" displayName="Table2" ref="A1:H79" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H79" xr:uid="{9D043231-9B53-AA48-9D06-6F5D5240F721}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H79">
     <sortCondition ref="A1:A79"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="10" xr3:uid="{CE02F916-E33E-9044-9F03-86A0123B521A}" name="Trip Key" dataDxfId="9">
+  <tableColumns count="8">
+    <tableColumn id="10" xr3:uid="{CE02F916-E33E-9044-9F03-86A0123B521A}" name="Trip Key" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT(B2,"-",C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{3E698417-7665-CE42-82EA-203FEA0B2676}" name="Trip" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{092C9153-3898-A14B-84B4-E5FBB6852C40}" name="Day" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{10269964-C810-0648-809E-B72746D168FA}" name="Leader" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{65A1D2D5-1A7B-684B-9AC4-CC1A03C3F486}" name="ebird lister" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4E18F06A-A744-4C4A-A64C-F8498DEB4442}" name="Done?" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{7BB502F6-8E98-0144-A559-B044192EA29E}" name="Trip Reports" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{F6EB316D-564A-864D-90C1-A5BB52763F04}" name="Checklists" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{DA9C5E18-65AB-2D4C-B6BC-7B3E697EF648}" name="Trip Report Compilation Output" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3E698417-7665-CE42-82EA-203FEA0B2676}" name="Trip" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{092C9153-3898-A14B-84B4-E5FBB6852C40}" name="Day" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{10269964-C810-0648-809E-B72746D168FA}" name="Leader" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{65A1D2D5-1A7B-684B-9AC4-CC1A03C3F486}" name="ebird lister" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4E18F06A-A744-4C4A-A64C-F8498DEB4442}" name="Done?" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{7BB502F6-8E98-0144-A559-B044192EA29E}" name="Trip Reports/Checklists" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{A3A457D4-13DF-9045-BEC2-40FD0BF6AF7F}" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1732,13 +1500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2376B23C-420E-EB4F-A835-9CB19BA67F1E}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1750,13 +1518,12 @@
     <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.83203125" customWidth="1"/>
     <col min="7" max="7" width="41.6640625" customWidth="1"/>
-    <col min="8" max="9" width="37.83203125" customWidth="1"/>
-    <col min="10" max="10" width="43.33203125" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>35</v>
@@ -1771,22 +1538,16 @@
         <v>40</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>44</v>
+        <v>261</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="str">
         <f t="shared" ref="A2:A31" si="0">_xlfn.CONCAT(B2,"-",C2)</f>
         <v>Ahtanum #2-Friday</v>
@@ -1798,24 +1559,20 @@
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Ahtanum-Friday</v>
@@ -1827,24 +1584,20 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>66</v>
+      <c r="G3" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Ahtanum-Saturday</v>
@@ -1860,16 +1613,12 @@
       <c r="F4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="8">
-        <v>394588</v>
+      <c r="G4" s="20" t="s">
+        <v>263</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Ahtanum-Sunday</v>
@@ -1881,24 +1630,20 @@
         <v>6</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Bethel Ridge Owls-Sunday</v>
@@ -1910,24 +1655,20 @@
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Bethel Ridge Owls-Thursday</v>
@@ -1939,24 +1680,20 @@
         <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>327</v>
+        <v>253</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Burrowing Owl  Tour-Friday</v>
@@ -1968,24 +1705,20 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Chinook Pass-Friday</v>
@@ -1997,22 +1730,18 @@
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="18" t="s">
-        <v>317</v>
+        <v>248</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Chinook Pass-Saturday</v>
@@ -2024,24 +1753,20 @@
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Chinook Pass-Sunday</v>
@@ -2053,135 +1778,117 @@
         <v>6</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="str">
+    </row>
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="str">
         <f t="shared" ref="A12:A14" si="1">_xlfn.CONCAT(B12,"-",C12)</f>
         <v>Coming Over:
 North Seattle / Snohomish Co-Thursday</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>333</v>
+        <v>255</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>337</v>
+        <v>259</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="str">
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Coming Over:
 Vancouver/Columbia Gorge-Thursday</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>334</v>
+        <v>256</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="str">
+    </row>
+    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Going Home:
 Chinook Pass-Monday</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>335</v>
+        <v>257</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>336</v>
+        <v>258</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>338</v>
+        <v>260</v>
       </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Cowiche Canyon 2-Sunday</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Cowiche Canyon-Friday</v>
@@ -2193,24 +1900,20 @@
         <v>2</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Cowiche Canyon-Sunday</v>
@@ -2222,24 +1925,20 @@
         <v>6</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Eschbach Nature Area &amp; Painted Rocks-Saturday</v>
@@ -2251,24 +1950,20 @@
         <v>5</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Eschbach Nature Area &amp; Painted Rocks-Sunday</v>
@@ -2280,24 +1975,20 @@
         <v>6</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G19" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Fort Simcoe State Park-Friday</v>
@@ -2309,24 +2000,20 @@
         <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Fort Simcoe State Park-Saturday</v>
@@ -2338,24 +2025,20 @@
         <v>5</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="G21" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Fort Simcoe State Park-Sunday</v>
@@ -2367,24 +2050,20 @@
         <v>6</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+      <c r="G22" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Hop Capitol Birds-n-Brews -Saturday</v>
@@ -2396,24 +2075,20 @@
         <v>5</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="I23" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Horse Heaven Hills-Saturday</v>
@@ -2425,24 +2100,20 @@
         <v>5</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Horse Heaven Hills-Sunday</v>
@@ -2454,24 +2125,20 @@
         <v>6</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H25" s="5"/>
-      <c r="I25" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Naneum-Colockum-Friday</v>
@@ -2483,22 +2150,18 @@
         <v>2</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>314</v>
+        <v>247</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" ht="280" customHeight="1" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" ht="280" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Naneum-Colockum-Saturday</v>
@@ -2510,26 +2173,22 @@
         <v>5</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G27" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Naneum-Colockum-Sunday</v>
@@ -2541,24 +2200,20 @@
         <v>6</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Nile &amp; Rattlesnake
@@ -2579,16 +2234,12 @@
       <c r="F29" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="9">
-        <v>387050</v>
+      <c r="G29" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Nile &amp; Rattlesnake
@@ -2604,21 +2255,17 @@
         <v>42</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="13">
-        <v>387044</v>
+      <c r="G30" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="H30" s="5"/>
-      <c r="I30" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Nile &amp; Rattlesnake
@@ -2631,22 +2278,18 @@
         <v>6</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="13">
-        <v>384698</v>
+      <c r="G31" s="9" t="s">
+        <v>266</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="str">
         <f t="shared" ref="A32:A63" si="2">_xlfn.CONCAT(B32,"-",C32)</f>
         <v>Oak Creek Canyon-Friday</v>
@@ -2658,22 +2301,18 @@
         <v>2</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Oak Creek Canyon-Saturday</v>
@@ -2685,26 +2324,20 @@
         <v>5</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G33" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Oak Creek Canyon-Sunday</v>
@@ -2716,24 +2349,20 @@
         <v>6</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Observatory Rd-Umtanum Falls-Sunday</v>
@@ -2747,16 +2376,12 @@
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="G35" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Photographer-Friendly -Saturday</v>
@@ -2768,24 +2393,20 @@
         <v>5</v>
       </c>
       <c r="D36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Quilomene-Wild Horse Wind Farm -Friday</v>
@@ -2797,24 +2418,20 @@
         <v>2</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="G37" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Quilomene-Wild Horse Wind Farm -Saturday</v>
@@ -2826,24 +2443,20 @@
         <v>5</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H38" s="5"/>
-      <c r="I38" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Quilomene-Wild Horse Wind Farm -Sunday</v>
@@ -2855,24 +2468,20 @@
         <v>6</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H39" s="5"/>
-      <c r="I39" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Rimrock Owls/Leader's Choice-Sunday</v>
@@ -2884,24 +2493,20 @@
         <v>6</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="G40" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Rimrock Owls/Leader's Choice-Thursday</v>
@@ -2913,24 +2518,20 @@
         <v>32</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H41" s="5"/>
-      <c r="I41" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Robinson Canyon-Friday</v>
@@ -2942,24 +2543,20 @@
         <v>2</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="I42" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Robinson Canyon-Saturday</v>
@@ -2971,24 +2568,20 @@
         <v>5</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G43" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Robinson Canyon-Sunday</v>
@@ -3000,59 +2593,51 @@
         <v>6</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>325</v>
+        <v>252</v>
       </c>
       <c r="H44" s="5"/>
-      <c r="I44" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Snow Mountain Ranch-Friday</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Snow Mountain Ranch-Saturday</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>5</v>
@@ -3062,39 +2647,33 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Snow Mountain Ranch-Sunday</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G47" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Sunnyside Wildlife Area-Friday</v>
@@ -3106,24 +2685,20 @@
         <v>2</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G48" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Sunnyside Wildlife Area-Saturday</v>
@@ -3135,24 +2710,20 @@
         <v>5</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H49" s="5"/>
-      <c r="I49" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Sunnyside Wildlife Area-Sunday</v>
@@ -3164,24 +2735,20 @@
         <v>6</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H50" s="5"/>
-      <c r="I50" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Taneum Creek-Saturday</v>
@@ -3193,24 +2760,20 @@
         <v>5</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H51" s="5"/>
-      <c r="I51" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Taneum Creek-Sunday</v>
@@ -3222,24 +2785,20 @@
         <v>6</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H52" s="5"/>
-      <c r="I52" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Teanaway-Friday</v>
@@ -3251,24 +2810,20 @@
         <v>2</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H53" s="5"/>
-      <c r="I53" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="J53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Teanaway-Saturday</v>
@@ -3280,24 +2835,20 @@
         <v>5</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H54" s="5"/>
-      <c r="I54" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Toppenish NWR-Friday</v>
@@ -3309,24 +2860,20 @@
         <v>2</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H55" s="5"/>
-      <c r="I55" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Toppenish NWR-Saturday</v>
@@ -3338,24 +2885,20 @@
         <v>5</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="J56" s="5"/>
-    </row>
-    <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="G56" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Toppenish NWR-Sunday</v>
@@ -3367,49 +2910,41 @@
         <v>6</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H57" s="5"/>
-      <c r="I57" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="J57" s="5"/>
-    </row>
-    <row r="58" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Umptanum Road-Wenas Loop #2-Sunday</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="6"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="J58" s="5"/>
-    </row>
-    <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G58" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Umptanum Road-Wenas Loop-Friday</v>
@@ -3421,24 +2956,20 @@
         <v>2</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H59" s="5"/>
-      <c r="I59" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Umptanum Road-Wenas Loop-Saturday</v>
@@ -3450,24 +2981,20 @@
         <v>5</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H60" s="5"/>
-      <c r="I60" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Umptanum Road-Wenas Loop-Sunday</v>
@@ -3479,24 +3006,20 @@
         <v>6</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H61" s="5"/>
-      <c r="I61" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="J61" s="5"/>
-    </row>
-    <row r="62" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Vantage, Wanapum &amp; Getty’s Cove-Friday</v>
@@ -3508,24 +3031,20 @@
         <v>2</v>
       </c>
       <c r="D62" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="H62" s="5"/>
-      <c r="I62" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Vantage, Wanapum &amp; Getty’s Cove-Sunday</v>
@@ -3537,7 +3056,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>43</v>
@@ -3546,15 +3065,11 @@
         <v>39</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H63" s="5"/>
-      <c r="I63" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="J63" s="5"/>
-    </row>
-    <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="str">
         <f t="shared" ref="A64:A79" si="3">_xlfn.CONCAT(B64,"-",C64)</f>
         <v>Wenas Owls -Sunday</v>
@@ -3570,10 +3085,8 @@
       <c r="F64" s="6"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Wenas Owls -Thursday</v>
@@ -3585,24 +3098,20 @@
         <v>32</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H65" s="5"/>
-      <c r="I65" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="str">
         <f t="shared" si="3"/>
         <v>White Pass West- SD-Saturday</v>
@@ -3614,24 +3123,20 @@
         <v>5</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H66" s="5"/>
-      <c r="I66" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
         <f t="shared" si="3"/>
         <v>White Pass West-Friday</v>
@@ -3643,24 +3148,20 @@
         <v>2</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H67" s="5"/>
-      <c r="I67" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="str">
         <f t="shared" si="3"/>
         <v>White Pass West-Saturday</v>
@@ -3672,24 +3173,20 @@
         <v>5</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H68" s="5"/>
-      <c r="I68" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="str">
         <f t="shared" si="3"/>
         <v>White Pass West-Sunday</v>
@@ -3701,24 +3198,20 @@
         <v>6</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H69" s="5"/>
-      <c r="I69" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakama Eagle-Bison Trip-Friday</v>
@@ -3730,24 +3223,20 @@
         <v>2</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>311</v>
+        <v>245</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>311</v>
+        <v>245</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>312</v>
+        <v>246</v>
       </c>
       <c r="H70" s="5"/>
-      <c r="I70" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima Greenway-Friday</v>
@@ -3759,24 +3248,20 @@
         <v>2</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H71" s="5"/>
-      <c r="I71" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima Greenway-Sunday</v>
@@ -3788,22 +3273,18 @@
         <v>6</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E72" s="7"/>
       <c r="F72" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="J72" s="5"/>
-    </row>
-    <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G72" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon Owls-Friday</v>
@@ -3815,24 +3296,20 @@
         <v>2</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H73" s="5"/>
-      <c r="I73" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="J73" s="5"/>
-    </row>
-    <row r="74" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon Owls-Sunday</v>
@@ -3844,24 +3321,20 @@
         <v>6</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H74" s="5"/>
-      <c r="I74" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="J74" s="5"/>
-    </row>
-    <row r="75" spans="1:10" ht="189" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:8" ht="189" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon-Driving-Friday</v>
@@ -3873,24 +3346,20 @@
         <v>2</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="J75" s="5"/>
-    </row>
-    <row r="76" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="G75" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon-Driving-Saturday</v>
@@ -3902,24 +3371,20 @@
         <v>5</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H76" s="5"/>
-      <c r="I76" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon-Driving-Sunday</v>
@@ -3931,24 +3396,20 @@
         <v>6</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H77" s="5"/>
-      <c r="I77" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="J77" s="5"/>
-    </row>
-    <row r="78" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon-Hike Umtanum Ck.-Friday</v>
@@ -3960,24 +3421,20 @@
         <v>2</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H78" s="5"/>
-      <c r="I78" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="J78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Yakima River Canyon-Hike Umtanum Ck.-Saturday</v>
@@ -3989,42 +3446,43 @@
         <v>5</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H79" s="5"/>
-      <c r="I79" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="J79" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G29" r:id="rId1" display="https://ebird.org/tripreport/387050" xr:uid="{89D9718D-94EB-B445-A633-638ECAA3EC00}"/>
+    <hyperlink ref="G29" r:id="rId1" xr:uid="{89D9718D-94EB-B445-A633-638ECAA3EC00}"/>
     <hyperlink ref="G77" r:id="rId2" xr:uid="{26DFAE62-C93A-104F-BD12-939282D7B849}"/>
     <hyperlink ref="G2" r:id="rId3" xr:uid="{BCFB4C54-0C11-B44A-B521-54EC7B271A01}"/>
-    <hyperlink ref="H48" r:id="rId4" xr:uid="{A23E4495-80F7-F145-BE79-BCCB385CA0B6}"/>
-    <hyperlink ref="H19" r:id="rId5" xr:uid="{B31D440E-68DB-0644-AB6C-AF6C3B6829C2}"/>
-    <hyperlink ref="G70" r:id="rId6" xr:uid="{13824842-E76D-264F-A4A0-A3D787EC27D4}"/>
-    <hyperlink ref="G9" r:id="rId7" xr:uid="{A27D4C09-8096-B042-9DF0-0875DA94329E}"/>
-    <hyperlink ref="H35" r:id="rId8" display="https://ebird.org/checklist/S248378222_x000a_https://ebird.org/checklist/S248378221_x000a_https://ebird.org/checklist/S248378219_x000a_https://ebird.org/checklist/S248378218_x000a_https://ebird.org/checklist/S248378217_x000a_https://ebird.org/checklist/S248378216_x000a_https://ebird.org/checklist/S248378214_x000a_https://ebird.org/checklist/S248616536_x000a_https://ebird.org/checklist/S248378260" xr:uid="{4FF2C337-F4AA-3F40-9E28-55595EA63D88}"/>
-    <hyperlink ref="G42" r:id="rId9" xr:uid="{47D16DC2-6C15-D642-B050-88A1B37B0C43}"/>
-    <hyperlink ref="G44" r:id="rId10" xr:uid="{8D123904-EF74-2E41-8705-53C65342B12F}"/>
-    <hyperlink ref="G7" r:id="rId11" xr:uid="{319923A8-2D35-1145-96C3-B9583DAC5952}"/>
-    <hyperlink ref="G12" r:id="rId12" xr:uid="{3533B44A-2625-0A46-93E3-360A44298DE1}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{92F69AC5-D741-1E42-8424-65FAF74C97B4}"/>
+    <hyperlink ref="G48" r:id="rId4" xr:uid="{A23E4495-80F7-F145-BE79-BCCB385CA0B6}"/>
+    <hyperlink ref="G70" r:id="rId5" xr:uid="{13824842-E76D-264F-A4A0-A3D787EC27D4}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{A27D4C09-8096-B042-9DF0-0875DA94329E}"/>
+    <hyperlink ref="G35" r:id="rId7" display="https://ebird.org/checklist/S248378222_x000a_https://ebird.org/checklist/S248378221_x000a_https://ebird.org/checklist/S248378219_x000a_https://ebird.org/checklist/S248378218_x000a_https://ebird.org/checklist/S248378217_x000a_https://ebird.org/checklist/S248378216_x000a_https://ebird.org/checklist/S248378214_x000a_https://ebird.org/checklist/S248616536_x000a_https://ebird.org/checklist/S248378260" xr:uid="{4FF2C337-F4AA-3F40-9E28-55595EA63D88}"/>
+    <hyperlink ref="G42" r:id="rId8" xr:uid="{47D16DC2-6C15-D642-B050-88A1B37B0C43}"/>
+    <hyperlink ref="G44" r:id="rId9" xr:uid="{8D123904-EF74-2E41-8705-53C65342B12F}"/>
+    <hyperlink ref="G7" r:id="rId10" xr:uid="{319923A8-2D35-1145-96C3-B9583DAC5952}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{3533B44A-2625-0A46-93E3-360A44298DE1}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{92F69AC5-D741-1E42-8424-65FAF74C97B4}"/>
+    <hyperlink ref="G19" r:id="rId13" xr:uid="{3DED9103-8ECF-7B4C-971A-FA705F799FCC}"/>
+    <hyperlink ref="G33" r:id="rId14" display="https://ebird.org/tripreport/382648," xr:uid="{FB9D9C01-AF46-BB49-8145-D6786B4D8612}"/>
+    <hyperlink ref="G3" r:id="rId15" xr:uid="{59C84B79-8F13-5746-BF21-4DE15B4A2694}"/>
+    <hyperlink ref="G4" r:id="rId16" xr:uid="{B7F6AEC3-D334-4342-941F-EC9512BEE402}"/>
+    <hyperlink ref="G30" r:id="rId17" xr:uid="{F4E82896-F0B9-8B47-9505-28586F3FE01C}"/>
+    <hyperlink ref="G31" r:id="rId18" xr:uid="{D1BD873B-DFF6-094E-8C50-6569A7B09427}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4085,57 +3543,57 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="G1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="N1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="P1" s="17" t="s">
         <v>148</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C2" s="16">
         <v>1</v>
@@ -4150,7 +3608,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C3" s="16">
         <v>1</v>
@@ -4165,7 +3623,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C4" s="16">
         <v>18</v>
@@ -4186,7 +3644,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C5" s="16">
         <v>10</v>
@@ -4207,7 +3665,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C6" s="16">
         <v>16</v>
@@ -4225,7 +3683,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7" s="16">
         <v>4</v>
@@ -4243,7 +3701,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C8" s="16">
         <v>4</v>
@@ -4258,7 +3716,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -4273,7 +3731,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C10" s="16">
         <v>4</v>
@@ -4291,7 +3749,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C11" s="16">
         <v>1</v>
@@ -4306,7 +3764,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C12" s="16">
         <v>2</v>
@@ -4321,7 +3779,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C13" s="16">
         <v>5</v>
@@ -4339,7 +3797,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="16" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C14" s="16">
         <v>2</v>
@@ -4354,7 +3812,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C15" s="16">
         <v>16</v>
@@ -4372,7 +3830,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C16" s="16">
         <v>5</v>
@@ -4393,7 +3851,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C17" s="16">
         <v>9</v>
@@ -4417,7 +3875,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
@@ -4432,7 +3890,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B19" s="16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C19" s="16">
         <v>1</v>
@@ -4447,7 +3905,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C20" s="16">
         <v>5</v>
@@ -4468,10 +3926,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C21" s="16">
         <v>2</v>
@@ -4489,7 +3947,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B22" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C22" s="16">
         <v>11</v>
@@ -4510,7 +3968,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B23" s="16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C23" s="16">
         <v>2</v>
@@ -4525,7 +3983,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C24" s="16">
         <v>14</v>
@@ -4555,7 +4013,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B25" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C25" s="16">
         <v>9</v>
@@ -4576,7 +4034,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B26" s="16" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C26" s="16">
         <v>1</v>
@@ -4591,7 +4049,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B27" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C27" s="16">
         <v>1</v>
@@ -4603,7 +4061,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B28" s="16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C28" s="16">
         <v>4</v>
@@ -4621,7 +4079,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B29" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C29" s="16">
         <v>2</v>
@@ -4636,7 +4094,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C30" s="16">
         <v>4</v>
@@ -4654,7 +4112,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C31" s="16">
         <v>14</v>
@@ -4681,7 +4139,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C32" s="16">
         <v>6</v>
@@ -4699,7 +4157,7 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C33" s="16">
         <v>15</v>
@@ -4720,7 +4178,7 @@
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C34" s="16">
         <v>1</v>
@@ -4735,7 +4193,7 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" s="16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C35" s="16">
         <v>10</v>
@@ -4762,7 +4220,7 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C36" s="16">
         <v>4</v>
@@ -4780,7 +4238,7 @@
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C37" s="16">
         <v>5</v>
@@ -4795,7 +4253,7 @@
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C38" s="16">
         <v>6</v>
@@ -4813,7 +4271,7 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="16" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C39" s="16">
         <v>8</v>
@@ -4834,7 +4292,7 @@
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C40" s="16">
         <v>5</v>
@@ -4852,7 +4310,7 @@
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" s="16" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C41" s="16">
         <v>8</v>
@@ -4870,7 +4328,7 @@
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C42" s="16">
         <v>1</v>
@@ -4885,7 +4343,7 @@
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C43" s="16">
         <v>2</v>
@@ -4900,7 +4358,7 @@
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B44" s="16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C44" s="16">
         <v>9</v>
@@ -4918,7 +4376,7 @@
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B45" s="16" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C45" s="16">
         <v>10</v>
@@ -4936,7 +4394,7 @@
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46" s="16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C46" s="15">
         <v>5</v>
@@ -4948,7 +4406,7 @@
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B47" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C47" s="16">
         <v>35</v>
@@ -4969,7 +4427,7 @@
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B48" s="16" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C48" s="16">
         <v>3</v>
@@ -4984,7 +4442,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B49" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C49" s="16">
         <v>4</v>
@@ -4999,7 +4457,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B50" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C50" s="16">
         <v>2</v>
@@ -5014,7 +4472,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B51" s="16" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C51" s="16">
         <v>2</v>
@@ -5032,7 +4490,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B52" s="16" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C52" s="16">
         <v>7</v>
@@ -5047,7 +4505,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B53" s="16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C53" s="16">
         <v>2</v>
@@ -5065,7 +4523,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B54" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C54" s="16">
         <v>25</v>
@@ -5098,7 +4556,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B55" s="16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C55" s="16">
         <v>16</v>
@@ -5119,7 +4577,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B56" s="16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C56" s="16">
         <v>10</v>
@@ -5134,7 +4592,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B57" s="16" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C57" s="16">
         <v>3</v>
@@ -5152,7 +4610,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B58" s="16" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C58" s="16">
         <v>8</v>
@@ -5170,7 +4628,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B59" s="16" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C59" s="16">
         <v>8</v>
@@ -5191,7 +4649,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B60" s="16" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C60" s="16">
         <v>2</v>
@@ -5206,7 +4664,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B61" s="16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C61" s="16">
         <v>10</v>
@@ -5230,7 +4688,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B62" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C62" s="16">
         <v>5</v>
@@ -5245,7 +4703,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B63" s="16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C63" s="16">
         <v>1</v>
@@ -5260,10 +4718,10 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C64" s="16">
         <v>1</v>
@@ -5278,7 +4736,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B65" s="16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C65" s="16">
         <v>2</v>
@@ -5293,10 +4751,10 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C66" s="16">
         <v>1</v>
@@ -5311,7 +4769,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B67" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C67" s="16">
         <v>3</v>
@@ -5326,7 +4784,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B68" s="16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C68" s="16">
         <v>1</v>
@@ -5341,7 +4799,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B69" s="16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C69" s="16">
         <v>3</v>
@@ -5359,7 +4817,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B70" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C70" s="16">
         <v>11</v>
@@ -5374,7 +4832,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B71" s="16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C71" s="16">
         <v>7</v>
@@ -5392,7 +4850,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B72" s="16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C72" s="16">
         <v>7</v>
@@ -5410,7 +4868,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B73" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C73" s="16">
         <v>15</v>
@@ -5431,7 +4889,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B74" s="16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C74" s="16">
         <v>2</v>
@@ -5446,7 +4904,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B75" s="16" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C75" s="16">
         <v>9</v>
@@ -5464,7 +4922,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C76" s="16">
         <v>9</v>
@@ -5482,7 +4940,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B77" s="16" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C77" s="16">
         <v>15</v>
@@ -5506,7 +4964,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B78" s="16" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C78" s="16">
         <v>2</v>
@@ -5521,7 +4979,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B79" s="16" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C79" s="16">
         <v>21</v>
@@ -5548,7 +5006,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B80" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C80" s="16">
         <v>4</v>
@@ -5566,7 +5024,7 @@
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B81" s="16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C81" s="16">
         <v>4</v>
@@ -5584,7 +5042,7 @@
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B82" s="16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C82" s="16">
         <v>1</v>
@@ -5599,7 +5057,7 @@
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B83" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C83" s="16">
         <v>4</v>
@@ -5617,7 +5075,7 @@
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B84" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C84" s="16">
         <v>6</v>
@@ -5641,7 +5099,7 @@
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B85" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C85" s="16">
         <v>19</v>
@@ -5671,7 +5129,7 @@
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B86" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C86" s="16">
         <v>1</v>

</xml_diff>